<commit_message>
- Particle plate table added - Side plates layout and thickness changed to make it stiffer and easier to find material - BOM updated
</commit_message>
<xml_diff>
--- a/docs/BOM.xlsx
+++ b/docs/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SVET\CNC3040\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SVET\CNC4060\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C77DDF-0A74-4911-94DA-3D3794EE5BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F385915-1123-46B5-93F8-473092CBEAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{55619F47-F0BA-4A13-8544-E1B0D0B31264}"/>
+    <workbookView xWindow="4957" yWindow="1815" windowWidth="20550" windowHeight="9278" xr2:uid="{55619F47-F0BA-4A13-8544-E1B0D0B31264}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Item name</t>
   </si>
@@ -48,72 +48,18 @@
     <t>Link</t>
   </si>
   <si>
-    <t>4080 extrusion</t>
-  </si>
-  <si>
     <t>in</t>
   </si>
   <si>
-    <t>https://8020.net/40-4080.html</t>
-  </si>
-  <si>
-    <t>https://8020.net/40-4012.html</t>
-  </si>
-  <si>
-    <t>40120 extrusion</t>
-  </si>
-  <si>
     <t>service price</t>
   </si>
   <si>
-    <t>VFD 3Hp</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Variable-Frequency-Inverter-Converter-HUANYANG/dp/B0775F4G47/ref=pd_sbs_7/142-0088220-7715321?pd_rd_w=5x1DU&amp;pf_rd_p=a5925d26-9630-40f3-a011-d858608ac88b&amp;pf_rd_r=NTFB8CQ5P2VCFZ5K0BQK&amp;pd_rd_r=28712fdc-4185-489d-a060-0a777d58e1e3&amp;pd_rd_wg=ShIq3&amp;pd_rd_i=B0775QGLVJ&amp;th=1</t>
-  </si>
-  <si>
     <t>pcs</t>
   </si>
   <si>
     <t>sfu1605 250mm set</t>
   </si>
   <si>
-    <t>https://www.amazon.com/250mm-Screw-SFU1605-Diameter-Machine/dp/B08QHYSK64/ref=sr_1_26?dchild=1&amp;keywords=sfu1605+250mm&amp;qid=1624385893&amp;sr=8-26</t>
-  </si>
-  <si>
-    <t>15x300 + 4 carriage</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Happybuy-15-300mm-Guideway-Carriage-Bearings/dp/B06X19RMC9/ref=cm_cr_arp_d_product_top?ie=UTF8</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Square-Linear-L1000mm-TRH20B-Carriage/dp/B07M8T1NG1/ref=sr_1_19?_encoding=UTF8&amp;c=ts&amp;dchild=1&amp;keywords=Linear%2BMotion%2BGuides&amp;qid=1624397154&amp;refinements=p_76%3A1249158011%2Cp_72%3A1248921011&amp;rnid=1248919011&amp;rps=1&amp;s=industrial&amp;sr=1-19&amp;ts_id=979107011&amp;th=1</t>
-  </si>
-  <si>
-    <t>TRH20x800 + 2 TRH20B</t>
-  </si>
-  <si>
-    <t>15x600 + 4 carriage</t>
-  </si>
-  <si>
-    <t>~100</t>
-  </si>
-  <si>
-    <t>sfu1605 600mm set</t>
-  </si>
-  <si>
-    <t>~60</t>
-  </si>
-  <si>
-    <t>sfu1605 400mm set</t>
-  </si>
-  <si>
-    <t>~50</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/dp/B08BWN8V7P?psc=1&amp;smid=AWADNQ91WGVYS&amp;ref_=chk_typ_imgToDp</t>
-  </si>
-  <si>
     <t>HGR20x300mm X 2 + 4xHGH20CA</t>
   </si>
   <si>
@@ -123,19 +69,79 @@
     <t>5/8" X 6" ALUMINUM 6061 FLAT BAR 12" Long</t>
   </si>
   <si>
-    <t>https://www.ebay.com/itm/360976433618?_trkparms=aid%3D111001%26algo%3DREC.SEED%26ao%3D1%26asc%3D20160908103841%26meid%3Dc03d699046454d76bd37efdb083735d2%26pid%3D100227%26rk%3D1%26rkt%3D15%26sd%3D360976433618%26itm%3D360976433618%26pmt%3D0%26noa%3D1%26pg%3D2053904&amp;_trksid=p2053904.c100227.m3827</t>
-  </si>
-  <si>
-    <t>steppers+drivers+psu</t>
-  </si>
-  <si>
-    <t>~300</t>
-  </si>
-  <si>
     <t>Controller PCB</t>
   </si>
   <si>
     <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>4HGR20x800 + 8 HGH20CA + 2sfu1605 800mm</t>
+  </si>
+  <si>
+    <t>sfu1605 550mm set</t>
+  </si>
+  <si>
+    <t>kit</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B08Q38TK1D</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07T6FKRBF</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/360976433618</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B08BWN8V7P</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B08QHYSK64</t>
+  </si>
+  <si>
+    <t>2x2in extrusion</t>
+  </si>
+  <si>
+    <t>2x4in extrusion</t>
+  </si>
+  <si>
+    <t>1/4 aluminum</t>
+  </si>
+  <si>
+    <t>Gantry plates 3/4 aluminum</t>
+  </si>
+  <si>
+    <t>1/2 back plate aluminum</t>
+  </si>
+  <si>
+    <t>extrusion (tatal price)</t>
+  </si>
+  <si>
+    <t>steppers</t>
+  </si>
+  <si>
+    <t>drivers</t>
+  </si>
+  <si>
+    <t>psu</t>
+  </si>
+  <si>
+    <t>router</t>
+  </si>
+  <si>
+    <t>screws</t>
+  </si>
+  <si>
+    <t>limit switches</t>
+  </si>
+  <si>
+    <t>router clamp</t>
+  </si>
+  <si>
+    <t>https://8020.net/2040-s.html</t>
+  </si>
+  <si>
+    <t>https://8020.net/2020-s.html</t>
   </si>
 </sst>
 </file>
@@ -218,15 +224,13 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -542,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B93920EF-7BFB-4544-A7B3-068DC985829A}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -566,11 +570,11 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="str">
-        <f>SUM(D2:D100) &amp; "$ already paid"</f>
-        <v>144.69$ already paid</v>
+        <f>SUM(D2:D94) &amp; "$ already paid"</f>
+        <v>373.19$ already paid</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -579,21 +583,21 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>1.1599999999999999</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="G2">
         <v>2.65</v>
@@ -601,171 +605,243 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>1.68</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G3">
         <v>2.65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>158</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2.61</v>
+      </c>
+      <c r="D4" s="3">
+        <v>39.61</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4">
-        <v>37</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2.61</v>
-      </c>
-      <c r="D5" s="4">
-        <v>39.61</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="B5" s="3">
+        <v>179.98</v>
+      </c>
+      <c r="C5" s="3">
+        <v>14.84</v>
+      </c>
+      <c r="D5" s="3">
+        <v>189.43</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3">
+        <v>36.090000000000003</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.98</v>
+      </c>
+      <c r="D6" s="3">
+        <v>39.07</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3.71</v>
+      </c>
+      <c r="D7" s="3">
+        <v>48.71</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3">
+        <v>46.99</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3.88</v>
+      </c>
+      <c r="D8" s="3">
+        <v>50.87</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>137</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="4">
-        <v>45</v>
-      </c>
-      <c r="C12" s="4">
-        <v>3.71</v>
-      </c>
-      <c r="D12" s="4">
-        <v>48.71</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="6" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="4">
-        <v>46.99</v>
-      </c>
-      <c r="C13" s="4">
-        <v>3.88</v>
-      </c>
-      <c r="D13" s="4">
-        <v>50.87</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="4">
-        <v>5.5</v>
-      </c>
-      <c r="D14" s="4">
-        <v>5.5</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>33</v>
+      <c r="B14">
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>31</v>
+      </c>
+      <c r="B21">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <f>SUM(B29:C29)</f>
+        <v>1242.19</v>
+      </c>
+      <c r="B29">
+        <f>SUM(B13:B23)</f>
+        <v>869</v>
+      </c>
+      <c r="C29">
+        <f>SUM(D2:D94)</f>
+        <v>373.19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" display="https://www.amazon.com/Square-Linear-L1000mm-TRH20B-Carriage/dp/B07M8T1NG1/ref=sr_1_19?_encoding=UTF8&amp;c=ts&amp;dchild=1&amp;keywords=Linear%2BMotion%2BGuides&amp;qid=1624397154&amp;refinements=p_76%3A1249158011%2Cp_72%3A1248921011&amp;rnid=1248919011&amp;rps=1&amp;s=industrial&amp;sr=1-19&amp;ts_id=979107011&amp;th=1" xr:uid="{78BAED14-119C-42E7-BE95-AD16BCF93CB1}"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{8F6F1F8D-F136-421C-A879-4770B92D3467}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{EFB17CEA-0D4E-4F15-8962-9605668A9B23}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{549AB7D9-57A1-41D4-8D42-3DB444D82B5D}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{4C888909-EC5F-4276-BE56-6638C66ED0B5}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{11FE077E-FF44-4439-B105-F3A48E3F4575}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- front plates added - Makita RT0701C spindle variant added - Frontplate on z-carriage was adjusted for new spindle variant
</commit_message>
<xml_diff>
--- a/docs/BOM.xlsx
+++ b/docs/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SVET\CNC4060\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7AB38B-9A88-4FB7-BE2B-2E9CFDFE3B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E025186A-E294-4738-9B1B-949F1ED03059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{55619F47-F0BA-4A13-8544-E1B0D0B31264}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{55619F47-F0BA-4A13-8544-E1B0D0B31264}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>Item name</t>
   </si>
@@ -96,15 +96,6 @@
     <t>https://www.amazon.com/gp/product/B08QHYSK64</t>
   </si>
   <si>
-    <t>1/4 aluminum</t>
-  </si>
-  <si>
-    <t>Gantry plates 3/4 aluminum</t>
-  </si>
-  <si>
-    <t>1/2 back plate aluminum</t>
-  </si>
-  <si>
     <t>steppers</t>
   </si>
   <si>
@@ -214,6 +205,30 @@
   </si>
   <si>
     <t>https://www.amazon.com/gp/product/B00E7D3V4S</t>
+  </si>
+  <si>
+    <t>3/4 aluminum flat 12"x16"</t>
+  </si>
+  <si>
+    <t>1/2 aluminum flat 2 1/2" x 30"</t>
+  </si>
+  <si>
+    <t>1/4 aluminum flat 4"x20"</t>
+  </si>
+  <si>
+    <t>shipping</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/usr/6061dude</t>
+  </si>
+  <si>
+    <t>electronics components for BB</t>
+  </si>
+  <si>
+    <t>Teensy 4.1</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com</t>
   </si>
 </sst>
 </file>
@@ -314,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -322,12 +337,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -345,6 +440,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -662,19 +766,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B93920EF-7BFB-4544-A7B3-068DC985829A}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="1" max="1" width="39.9296875" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="7.73046875" customWidth="1"/>
+    <col min="1" max="1" width="39.90625" customWidth="1"/>
+    <col min="2" max="2" width="17.6796875" customWidth="1"/>
+    <col min="3" max="3" width="7.7265625" customWidth="1"/>
     <col min="4" max="4" width="32.1328125" customWidth="1"/>
-    <col min="5" max="5" width="66.796875" customWidth="1"/>
-    <col min="6" max="6" width="45.73046875" customWidth="1"/>
-    <col min="7" max="7" width="15.59765625" customWidth="1"/>
+    <col min="5" max="5" width="66.76953125" customWidth="1"/>
+    <col min="6" max="6" width="45.7265625" customWidth="1"/>
+    <col min="7" max="7" width="15.58984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -689,7 +793,7 @@
       </c>
       <c r="D1" s="1" t="str">
         <f>SUM(D2:D85) &amp; "$ already paid"</f>
-        <v>660.24$ already paid</v>
+        <v>840.62$ already paid</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -812,9 +916,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="15.5" thickBot="1">
       <c r="A8" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2">
         <v>80</v>
@@ -826,90 +930,141 @@
         <v>86.8</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1">
+      <c r="A9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="13">
+        <v>62.54</v>
+      </c>
+      <c r="C9" s="13">
+        <v>9.94</v>
+      </c>
+      <c r="D9" s="14">
+        <v>130.38</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1">
+      <c r="A10" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="11">
+        <v>17.64</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="18"/>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1">
+      <c r="A11" s="15" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10">
+      <c r="B11" s="11">
+        <v>9.99</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="18"/>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="15.5" thickBot="1">
+      <c r="A12" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="17">
+        <v>30.27</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="19"/>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1">
+      <c r="A13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="11">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2">
+        <v>20</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1">
+      <c r="A14" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="11">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2">
+        <v>30</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B11">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17">
+      <c r="B22">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
         <f>SUM(B23:C23)</f>
-        <v>1138.2399999999998</v>
+        <v>1173.6200000000001</v>
       </c>
       <c r="B23">
-        <f>SUM(B10:B17)</f>
-        <v>478</v>
+        <f>SUM(B18:B22)</f>
+        <v>333</v>
       </c>
       <c r="C23">
         <f>SUM(D2:D85)</f>
-        <v>660.2399999999999</v>
+        <v>840.62000000000012</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1">
       <c r="A28" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B28" s="7">
         <v>0.12</v>
@@ -922,12 +1077,12 @@
         <v>9.84</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B29" s="8">
         <v>0.05</v>
@@ -940,12 +1095,12 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B30" s="8">
         <v>0.05</v>
@@ -958,12 +1113,12 @@
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1">
       <c r="A31" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B31" s="9">
         <v>0.12</v>
@@ -976,12 +1131,12 @@
         <v>0.96</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="2" customFormat="1">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B32" s="8">
         <v>0.12</v>
@@ -994,12 +1149,12 @@
         <v>9.84</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1">
       <c r="A33" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B33" s="8">
         <v>0.16</v>
@@ -1012,12 +1167,12 @@
         <v>5.12</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1">
       <c r="A34" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B34" s="8">
         <v>0.24</v>
@@ -1030,12 +1185,12 @@
         <v>4.8</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1">
       <c r="A35" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B35" s="9">
         <v>0.08</v>
@@ -1048,12 +1203,12 @@
         <v>0.64</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B36" s="9">
         <v>0.13</v>
@@ -1066,12 +1221,12 @@
         <v>2.8600000000000003</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1">
       <c r="A37" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B37" s="9">
         <v>0.12</v>
@@ -1084,12 +1239,12 @@
         <v>5.76</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1">
       <c r="A38" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B38" s="9">
         <v>0.25</v>
@@ -1102,12 +1257,12 @@
         <v>6</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1">
       <c r="A39" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B39" s="8">
         <v>0.09</v>
@@ -1120,12 +1275,12 @@
         <v>1.08</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="2" customFormat="1">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B40" s="8">
         <v>0.12</v>
@@ -1138,12 +1293,12 @@
         <v>2.88</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="2" customFormat="1">
       <c r="A41" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B41" s="8">
         <v>0.14000000000000001</v>
@@ -1156,17 +1311,17 @@
         <v>4.2</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="2" customFormat="1">
       <c r="A44" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="2" customFormat="1">
       <c r="A45" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B45" s="2">
         <v>27.7</v>
@@ -1178,12 +1333,12 @@
         <v>55.4</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="2" customFormat="1">
       <c r="A46" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B46" s="2">
         <v>12.5</v>
@@ -1195,12 +1350,12 @@
         <v>25</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="2" customFormat="1">
       <c r="A47" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B47" s="2">
         <v>9</v>
@@ -1212,12 +1367,12 @@
         <v>36</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="2" customFormat="1">
       <c r="A48" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D48" s="2">
         <v>26.67</v>
@@ -1231,8 +1386,11 @@
     <hyperlink ref="F5" r:id="rId4" xr:uid="{4C888909-EC5F-4276-BE56-6638C66ED0B5}"/>
     <hyperlink ref="F2" r:id="rId5" xr:uid="{11FE077E-FF44-4439-B105-F3A48E3F4575}"/>
     <hyperlink ref="F8" r:id="rId6" xr:uid="{32E600E3-8A62-4E72-AC9A-94BBC7765738}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{69B6F8A5-BE91-41C3-B3CC-0768F0E00B71}"/>
+    <hyperlink ref="F13" r:id="rId8" xr:uid="{66F4D46F-4E74-40C4-8D39-FE3B8678B641}"/>
+    <hyperlink ref="F14" r:id="rId9" xr:uid="{0DAD41F5-1BF9-41B9-B33C-50955157A63E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- limit sensors added - BOM updated
</commit_message>
<xml_diff>
--- a/docs/BOM.xlsx
+++ b/docs/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SVET\CNC4060\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E025186A-E294-4738-9B1B-949F1ED03059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C81FE96-F6D7-4079-8C8C-832417A31B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{55619F47-F0BA-4A13-8544-E1B0D0B31264}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{55619F47-F0BA-4A13-8544-E1B0D0B31264}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
   <si>
     <t>Item name</t>
   </si>
@@ -102,9 +102,6 @@
     <t>drivers</t>
   </si>
   <si>
-    <t>psu</t>
-  </si>
-  <si>
     <t>limit switches</t>
   </si>
   <si>
@@ -229,13 +226,52 @@
   </si>
   <si>
     <t>https://www.mouser.com</t>
+  </si>
+  <si>
+    <t>Limit switches 3pcs</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07V4PR84Y</t>
+  </si>
+  <si>
+    <t>Stepper drivers 2pcs DM556</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07WRR2HS6</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B091K5XS71</t>
+  </si>
+  <si>
+    <t>Steppers Nema 23 269oz-in 2pcs</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B081MX4PDC</t>
+  </si>
+  <si>
+    <t>Power supply 48V 600W</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B079D916WY</t>
+  </si>
+  <si>
+    <t>Collect reducer</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07WNNV1BW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSR 25A 2pcs </t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07QJ9KHHZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,27 +318,16 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF373736"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF373736"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF373736"/>
-      <name val="Inherit"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF373736"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -422,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -435,11 +460,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -449,6 +469,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -764,24 +792,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B93920EF-7BFB-4544-A7B3-068DC985829A}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="39.90625" customWidth="1"/>
-    <col min="2" max="2" width="17.6796875" customWidth="1"/>
-    <col min="3" max="3" width="7.7265625" customWidth="1"/>
+    <col min="1" max="1" width="39.9296875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="7.73046875" customWidth="1"/>
     <col min="4" max="4" width="32.1328125" customWidth="1"/>
-    <col min="5" max="5" width="66.76953125" customWidth="1"/>
-    <col min="6" max="6" width="45.7265625" customWidth="1"/>
-    <col min="7" max="7" width="15.58984375" customWidth="1"/>
+    <col min="5" max="5" width="66.796875" customWidth="1"/>
+    <col min="6" max="6" width="45.73046875" customWidth="1"/>
+    <col min="7" max="7" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,8 +820,8 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="str">
-        <f>SUM(D2:D85) &amp; "$ already paid"</f>
-        <v>840.62$ already paid</v>
+        <f>SUM(D2:D86) &amp; "$ already paid"</f>
+        <v>1036.8$ already paid</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -805,11 +833,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="7">
         <v>37</v>
       </c>
       <c r="C2" s="2">
@@ -825,11 +853,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="7">
         <v>179.98</v>
       </c>
       <c r="C3" s="2">
@@ -845,11 +873,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1">
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="7">
         <v>36.090000000000003</v>
       </c>
       <c r="C4" s="2">
@@ -865,11 +893,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1">
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="7">
         <v>45</v>
       </c>
       <c r="C5" s="2">
@@ -885,11 +913,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1">
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="7">
         <v>46.99</v>
       </c>
       <c r="C6" s="2">
@@ -902,11 +930,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1">
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="7">
         <v>5.5</v>
       </c>
       <c r="D7" s="2">
@@ -916,11 +944,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="15.5" thickBot="1">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="2">
+        <v>54</v>
+      </c>
+      <c r="B8" s="7">
         <v>80</v>
       </c>
       <c r="C8" s="2">
@@ -930,451 +958,556 @@
         <v>86.8</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" s="2" customFormat="1">
-      <c r="A9" s="12" t="s">
+      <c r="B9" s="17">
+        <v>62.54</v>
+      </c>
+      <c r="C9" s="10">
+        <v>9.94</v>
+      </c>
+      <c r="D9" s="11">
+        <v>130.38</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="13">
-        <v>62.54</v>
-      </c>
-      <c r="C9" s="13">
-        <v>9.94</v>
-      </c>
-      <c r="D9" s="14">
-        <v>130.38</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="B10" s="18">
+        <v>17.64</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="18">
+        <v>9.99</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="19">
+        <v>30.27</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" s="2" customFormat="1">
-      <c r="A10" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="11">
-        <v>17.64</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="18"/>
-    </row>
-    <row r="11" spans="1:7" s="2" customFormat="1">
-      <c r="A11" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="11">
-        <v>9.99</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="18"/>
-    </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="15.5" thickBot="1">
-      <c r="A12" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="17">
-        <v>30.27</v>
-      </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="19"/>
-    </row>
-    <row r="13" spans="1:7" s="2" customFormat="1">
-      <c r="A13" s="11" t="s">
+      <c r="B13" s="18">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2">
+        <v>25</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="11">
-        <v>20</v>
-      </c>
-      <c r="D13" s="2">
-        <v>20</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="2" customFormat="1">
-      <c r="A14" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="11">
+      <c r="B14" s="18">
         <v>30</v>
       </c>
       <c r="D14" s="2">
         <v>30</v>
       </c>
       <c r="F14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
+      <c r="B15" s="18">
+        <v>10.99</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="D15" s="2">
+        <v>11.9</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="18">
+        <v>29.98</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2.48</v>
+      </c>
+      <c r="D16" s="8">
+        <v>32.46</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="18">
+        <v>25.99</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2.15</v>
+      </c>
+      <c r="D17" s="8">
+        <v>28.14</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="18">
+        <v>40.99</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3.38</v>
+      </c>
+      <c r="D18" s="8">
+        <v>44.37</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="18">
+        <v>51.98</v>
+      </c>
+      <c r="C19" s="2">
+        <v>4.29</v>
+      </c>
+      <c r="D19" s="8">
+        <v>56.27</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="18">
+        <v>6.69</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D20" s="8">
+        <v>7.24</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="18">
+        <v>9.99</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="D21" s="8">
+        <v>10.8</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="20">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B18">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
+      <c r="B25" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <f>SUM(B26:C26)</f>
+        <v>1137.8000000000002</v>
+      </c>
+      <c r="B26" s="20">
+        <f>SUM(B23:B25)</f>
+        <v>101</v>
+      </c>
+      <c r="C26">
+        <f>SUM(D2:D86)</f>
+        <v>1036.8000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
-        <f>SUM(B23:C23)</f>
-        <v>1173.6200000000001</v>
-      </c>
-      <c r="B23">
-        <f>SUM(B18:B22)</f>
-        <v>333</v>
-      </c>
-      <c r="C23">
-        <f>SUM(D2:D85)</f>
-        <v>840.62000000000012</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="2" customFormat="1">
-      <c r="A28" s="6" t="s">
+      <c r="B29" s="21">
+        <v>0.12</v>
+      </c>
+      <c r="C29" s="2">
+        <v>82</v>
+      </c>
+      <c r="D29" s="2">
+        <f>B29*C29</f>
+        <v>9.84</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="7">
-        <v>0.12</v>
-      </c>
-      <c r="C28" s="2">
-        <v>82</v>
-      </c>
-      <c r="D28" s="2">
-        <f>B28*C28</f>
-        <v>9.84</v>
-      </c>
-      <c r="E28" s="2" t="s">
+    </row>
+    <row r="30" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" s="2" customFormat="1">
-      <c r="A29" s="2" t="s">
+      <c r="B30" s="21">
+        <v>0.05</v>
+      </c>
+      <c r="C30" s="2">
+        <v>24</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" ref="D30:D42" si="0">B30*C30</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B31" s="21">
         <v>0.05</v>
       </c>
-      <c r="C29" s="2">
-        <v>24</v>
-      </c>
-      <c r="D29" s="2">
-        <f t="shared" ref="D29:D41" si="0">B29*C29</f>
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="2" customFormat="1">
-      <c r="A30" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="C30" s="2">
+      <c r="C31" s="2">
         <v>40</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="2" customFormat="1">
-      <c r="A31" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="9">
+      <c r="E31" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="22">
         <v>0.12</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C32" s="2">
         <v>8</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>0.96</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="2" customFormat="1">
-      <c r="A32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="8">
+      <c r="E32" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="21">
         <v>0.12</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C33" s="2">
         <v>82</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>9.84</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="2" customFormat="1">
-      <c r="A33" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="8">
+      <c r="E33" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="21">
         <v>0.16</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C34" s="2">
         <v>32</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>5.12</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="2" customFormat="1">
-      <c r="A34" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="8">
+      <c r="E34" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="21">
         <v>0.24</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C35" s="2">
         <v>20</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="2" customFormat="1">
-      <c r="A35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="9">
+      <c r="E35" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="22">
         <v>0.08</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C36" s="2">
         <v>8</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>0.64</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="2" customFormat="1">
-      <c r="A36" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="9">
+      <c r="E36" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="22">
         <v>0.13</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C37" s="2">
         <v>22</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>2.8600000000000003</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="2" customFormat="1">
-      <c r="A37" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="9">
+      <c r="E37" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="22">
         <v>0.12</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C38" s="2">
         <v>48</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>5.76</v>
       </c>
-      <c r="E37" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="2" customFormat="1">
-      <c r="A38" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="9">
+      <c r="E38" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="22">
         <v>0.25</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C39" s="2">
         <v>24</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="2" customFormat="1">
-      <c r="A39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="8">
+      <c r="E39" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="21">
         <v>0.09</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C40" s="2">
         <v>12</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>1.08</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="2" customFormat="1">
-      <c r="A40" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="8">
+      <c r="E40" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="21">
         <v>0.12</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C41" s="2">
         <v>24</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>2.88</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="2" customFormat="1">
-      <c r="A41" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="8">
+      <c r="E41" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="21">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C42" s="2">
         <v>30</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="2" customFormat="1">
-      <c r="A44" s="2" t="s">
+      <c r="E42" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="7"/>
+    </row>
+    <row r="46" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" s="2" customFormat="1">
-      <c r="A45" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="2">
+      <c r="B46" s="7">
         <v>27.7</v>
-      </c>
-      <c r="C45" s="2">
-        <v>2</v>
-      </c>
-      <c r="D45" s="2">
-        <v>55.4</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="2" customFormat="1">
-      <c r="A46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="2">
-        <v>12.5</v>
       </c>
       <c r="C46" s="2">
         <v>2</v>
       </c>
       <c r="D46" s="2">
+        <v>55.4</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="7">
+        <v>12.5</v>
+      </c>
+      <c r="C47" s="2">
+        <v>2</v>
+      </c>
+      <c r="D47" s="2">
         <v>25</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E47" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" s="2" customFormat="1">
-      <c r="A47" s="2" t="s">
+      <c r="B48" s="7">
+        <v>9</v>
+      </c>
+      <c r="C48" s="2">
+        <v>4</v>
+      </c>
+      <c r="D48" s="2">
+        <v>36</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="2">
-        <v>9</v>
-      </c>
-      <c r="C47" s="2">
-        <v>4</v>
-      </c>
-      <c r="D47" s="2">
-        <v>36</v>
-      </c>
-      <c r="E47" s="2" t="s">
+    </row>
+    <row r="49" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" s="2" customFormat="1">
-      <c r="A48" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D48" s="2">
+      <c r="B49" s="7"/>
+      <c r="D49" s="2">
         <v>26.67</v>
       </c>
     </row>
@@ -1389,8 +1522,14 @@
     <hyperlink ref="F9" r:id="rId7" xr:uid="{69B6F8A5-BE91-41C3-B3CC-0768F0E00B71}"/>
     <hyperlink ref="F13" r:id="rId8" xr:uid="{66F4D46F-4E74-40C4-8D39-FE3B8678B641}"/>
     <hyperlink ref="F14" r:id="rId9" xr:uid="{0DAD41F5-1BF9-41B9-B33C-50955157A63E}"/>
+    <hyperlink ref="F15" r:id="rId10" xr:uid="{F0C9370C-25A3-4257-A175-04E90E8C4CED}"/>
+    <hyperlink ref="F16" r:id="rId11" xr:uid="{3DD7A837-C75A-4972-B66A-CCCC88EB2AC7}"/>
+    <hyperlink ref="F17" r:id="rId12" xr:uid="{8BE8DD27-9165-4039-BF3B-4475D47AF58C}"/>
+    <hyperlink ref="F19" r:id="rId13" xr:uid="{3A0A4360-124F-4360-B903-456534C8970A}"/>
+    <hyperlink ref="F18" r:id="rId14" xr:uid="{06F74424-E8E5-4284-BA67-C92524E17223}"/>
+    <hyperlink ref="F21" r:id="rId15" xr:uid="{95F47FF7-58F5-4E46-9CC7-4DC5699F57DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>